<commit_message>
Them chinh sua hoa don
</commit_message>
<xml_diff>
--- a/asset/HoaDon/template.xlsx
+++ b/asset/HoaDon/template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phungvantung/NetBeansProjects/ProjectMilkFE/asset/HoaDon/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phungvantung/NetBeansProjects/thithu/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F378F2CE-89F8-CA4F-AFC3-ECDF99B7A8B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541F4E96-90A9-7249-9CFD-DA068F85C66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>TT</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>THÀNH TIỀN</t>
-  </si>
-  <si>
-    <t>TỔNG CỘNG</t>
   </si>
   <si>
     <t>TÊN CỬA HÀNG: MilkFE</t>
@@ -66,7 +63,7 @@
     <t>Số điện thoại khách hàng:</t>
   </si>
   <si>
-    <t xml:space="preserve">Thời gian tạo : </t>
+    <t>Thời gian tạo hoá đơn :</t>
   </si>
 </sst>
 </file>
@@ -76,7 +73,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -120,24 +117,11 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -155,36 +139,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -292,76 +252,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -383,11 +278,50 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -395,101 +329,26 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -706,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA984"/>
+  <dimension ref="A1:AA985"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -724,140 +583,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="27"/>
+    </row>
+    <row r="2" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="39"/>
-    </row>
-    <row r="2" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18"/>
+    </row>
+    <row r="3" spans="1:27" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="25"/>
-    </row>
-    <row r="3" spans="1:27" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="30"/>
+    </row>
+    <row r="4" spans="1:27" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="18"/>
+    </row>
+    <row r="5" spans="1:27" s="7" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="18"/>
+    </row>
+    <row r="6" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="18"/>
+    </row>
+    <row r="7" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="22"/>
-    </row>
-    <row r="4" spans="1:27" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="18"/>
+    </row>
+    <row r="8" spans="1:27" ht="8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="12"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="13"/>
+    </row>
+    <row r="9" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
-    </row>
-    <row r="5" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="27"/>
-    </row>
-    <row r="6" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="42"/>
-    </row>
-    <row r="7" spans="1:27" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="28"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="29"/>
-    </row>
-    <row r="8" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="31" t="s">
+      <c r="F9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
-    </row>
-    <row r="9" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="33"/>
-    </row>
-    <row r="10" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="36"/>
-    </row>
-    <row r="11" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-    </row>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+    </row>
+    <row r="10" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="C12" s="6"/>
@@ -867,7 +712,7 @@
     <row r="13" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="C13" s="6"/>
-      <c r="D13" s="4"/>
+      <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -877,71 +722,71 @@
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="A15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
     </row>
     <row r="17" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+    </row>
+    <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="11"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
     </row>
     <row r="21" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
     </row>
     <row r="22" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="11"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="A22" s="3"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="11"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
     </row>
     <row r="24" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
     </row>
     <row r="25" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
@@ -6703,24 +6548,29 @@
       <c r="D984" s="4"/>
       <c r="E984" s="4"/>
     </row>
+    <row r="985" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A985" s="3"/>
+      <c r="C985" s="4"/>
+      <c r="D985" s="4"/>
+      <c r="E985" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="15">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A6:F6"/>
     <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A7:F7"/>
     <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A24:E24"/>
     <mergeCell ref="A16:E16"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="A17:E17"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:E20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape"/>

</xml_diff>